<commit_message>
Agregando el casting para el DTO con los resultados de las pruebas en el ThreadLocal
</commit_message>
<xml_diff>
--- a/sf_tests/src/test/resources/file.xlsx
+++ b/sf_tests/src/test/resources/file.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CasaM97\IdeaProjects\Selenium_Framework\sf_tests\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A8F18DA-D4B7-4A0D-A848-EBFDE104E371}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0438C236-9359-4E6E-97B7-713348C3EBFB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
   <si>
     <t>TEST CASE</t>
   </si>
@@ -43,6 +43,18 @@
   </si>
   <si>
     <t>Tecnología</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>Samsung Galaxy</t>
+  </si>
+  <si>
+    <t>Iphone</t>
   </si>
 </sst>
 </file>
@@ -361,10 +373,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -396,6 +408,28 @@
         <v>5</v>
       </c>
     </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Ajustes al TestManager para que pueda agregar al hilo instancias de nuevos objetos
</commit_message>
<xml_diff>
--- a/sf_tests/src/test/resources/file.xlsx
+++ b/sf_tests/src/test/resources/file.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CasaM97\IdeaProjects\Selenium_Framework\sf_tests\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0438C236-9359-4E6E-97B7-713348C3EBFB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99A7A3C1-56FE-454B-841E-F8B7D04D7D66}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="113">
   <si>
     <t>TEST CASE</t>
   </si>
@@ -55,16 +55,331 @@
   </si>
   <si>
     <t>Iphone</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>16</t>
+  </si>
+  <si>
+    <t>17</t>
+  </si>
+  <si>
+    <t>18</t>
+  </si>
+  <si>
+    <t>19</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>21</t>
+  </si>
+  <si>
+    <t>22</t>
+  </si>
+  <si>
+    <t>23</t>
+  </si>
+  <si>
+    <t>24</t>
+  </si>
+  <si>
+    <t>25</t>
+  </si>
+  <si>
+    <t>26</t>
+  </si>
+  <si>
+    <t>27</t>
+  </si>
+  <si>
+    <t>28</t>
+  </si>
+  <si>
+    <t>29</t>
+  </si>
+  <si>
+    <t>30</t>
+  </si>
+  <si>
+    <t>31</t>
+  </si>
+  <si>
+    <t>32</t>
+  </si>
+  <si>
+    <t>33</t>
+  </si>
+  <si>
+    <t>34</t>
+  </si>
+  <si>
+    <t>35</t>
+  </si>
+  <si>
+    <t>36</t>
+  </si>
+  <si>
+    <t>37</t>
+  </si>
+  <si>
+    <t>38</t>
+  </si>
+  <si>
+    <t>39</t>
+  </si>
+  <si>
+    <t>40</t>
+  </si>
+  <si>
+    <t>41</t>
+  </si>
+  <si>
+    <t>42</t>
+  </si>
+  <si>
+    <t>43</t>
+  </si>
+  <si>
+    <t>44</t>
+  </si>
+  <si>
+    <t>45</t>
+  </si>
+  <si>
+    <t>46</t>
+  </si>
+  <si>
+    <t>47</t>
+  </si>
+  <si>
+    <t>48</t>
+  </si>
+  <si>
+    <t>49</t>
+  </si>
+  <si>
+    <t>50</t>
+  </si>
+  <si>
+    <t>51</t>
+  </si>
+  <si>
+    <t>52</t>
+  </si>
+  <si>
+    <t>53</t>
+  </si>
+  <si>
+    <t>54</t>
+  </si>
+  <si>
+    <t>55</t>
+  </si>
+  <si>
+    <t>56</t>
+  </si>
+  <si>
+    <t>57</t>
+  </si>
+  <si>
+    <t>58</t>
+  </si>
+  <si>
+    <t>59</t>
+  </si>
+  <si>
+    <t>60</t>
+  </si>
+  <si>
+    <t>61</t>
+  </si>
+  <si>
+    <t>62</t>
+  </si>
+  <si>
+    <t>63</t>
+  </si>
+  <si>
+    <t>64</t>
+  </si>
+  <si>
+    <t>65</t>
+  </si>
+  <si>
+    <t>66</t>
+  </si>
+  <si>
+    <t>67</t>
+  </si>
+  <si>
+    <t>68</t>
+  </si>
+  <si>
+    <t>69</t>
+  </si>
+  <si>
+    <t>70</t>
+  </si>
+  <si>
+    <t>71</t>
+  </si>
+  <si>
+    <t>72</t>
+  </si>
+  <si>
+    <t>73</t>
+  </si>
+  <si>
+    <t>74</t>
+  </si>
+  <si>
+    <t>75</t>
+  </si>
+  <si>
+    <t>76</t>
+  </si>
+  <si>
+    <t>77</t>
+  </si>
+  <si>
+    <t>78</t>
+  </si>
+  <si>
+    <t>79</t>
+  </si>
+  <si>
+    <t>80</t>
+  </si>
+  <si>
+    <t>81</t>
+  </si>
+  <si>
+    <t>82</t>
+  </si>
+  <si>
+    <t>83</t>
+  </si>
+  <si>
+    <t>84</t>
+  </si>
+  <si>
+    <t>85</t>
+  </si>
+  <si>
+    <t>86</t>
+  </si>
+  <si>
+    <t>87</t>
+  </si>
+  <si>
+    <t>88</t>
+  </si>
+  <si>
+    <t>89</t>
+  </si>
+  <si>
+    <t>90</t>
+  </si>
+  <si>
+    <t>91</t>
+  </si>
+  <si>
+    <t>92</t>
+  </si>
+  <si>
+    <t>93</t>
+  </si>
+  <si>
+    <t>94</t>
+  </si>
+  <si>
+    <t>95</t>
+  </si>
+  <si>
+    <t>96</t>
+  </si>
+  <si>
+    <t>97</t>
+  </si>
+  <si>
+    <t>98</t>
+  </si>
+  <si>
+    <t>99</t>
+  </si>
+  <si>
+    <t>android</t>
+  </si>
+  <si>
+    <t>play station</t>
+  </si>
+  <si>
+    <t>xbox</t>
+  </si>
+  <si>
+    <t>wii</t>
+  </si>
+  <si>
+    <t>switch</t>
+  </si>
+  <si>
+    <t>laptop</t>
+  </si>
+  <si>
+    <t>smart tv</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -373,10 +688,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="B92" sqref="B92:B101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -430,7 +745,1075 @@
         <v>5</v>
       </c>
     </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" t="s">
+        <v>106</v>
+      </c>
+      <c r="C5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" t="s">
+        <v>107</v>
+      </c>
+      <c r="C6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" t="s">
+        <v>108</v>
+      </c>
+      <c r="C7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" t="s">
+        <v>109</v>
+      </c>
+      <c r="C8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" t="s">
+        <v>110</v>
+      </c>
+      <c r="C9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" t="s">
+        <v>111</v>
+      </c>
+      <c r="C10" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" t="s">
+        <v>112</v>
+      </c>
+      <c r="C11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" t="s">
+        <v>4</v>
+      </c>
+      <c r="C12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B15" t="s">
+        <v>106</v>
+      </c>
+      <c r="C15" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B16" t="s">
+        <v>107</v>
+      </c>
+      <c r="C16" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B17" t="s">
+        <v>108</v>
+      </c>
+      <c r="C17" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B18" t="s">
+        <v>109</v>
+      </c>
+      <c r="C18" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B19" t="s">
+        <v>110</v>
+      </c>
+      <c r="C19" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B20" t="s">
+        <v>111</v>
+      </c>
+      <c r="C20" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B21" t="s">
+        <v>112</v>
+      </c>
+      <c r="C21" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B22" t="s">
+        <v>4</v>
+      </c>
+      <c r="C22" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B23" t="s">
+        <v>8</v>
+      </c>
+      <c r="C23" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B24" t="s">
+        <v>9</v>
+      </c>
+      <c r="C24" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B25" t="s">
+        <v>106</v>
+      </c>
+      <c r="C25" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B26" t="s">
+        <v>107</v>
+      </c>
+      <c r="C26" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B27" t="s">
+        <v>108</v>
+      </c>
+      <c r="C27" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B28" t="s">
+        <v>109</v>
+      </c>
+      <c r="C28" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B29" t="s">
+        <v>110</v>
+      </c>
+      <c r="C29" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B30" t="s">
+        <v>111</v>
+      </c>
+      <c r="C30" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B31" t="s">
+        <v>112</v>
+      </c>
+      <c r="C31" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B32" t="s">
+        <v>4</v>
+      </c>
+      <c r="C32" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B33" t="s">
+        <v>8</v>
+      </c>
+      <c r="C33" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B34" t="s">
+        <v>9</v>
+      </c>
+      <c r="C34" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B35" t="s">
+        <v>106</v>
+      </c>
+      <c r="C35" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B36" t="s">
+        <v>107</v>
+      </c>
+      <c r="C36" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B37" t="s">
+        <v>108</v>
+      </c>
+      <c r="C37" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B38" t="s">
+        <v>109</v>
+      </c>
+      <c r="C38" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B39" t="s">
+        <v>110</v>
+      </c>
+      <c r="C39" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B40" t="s">
+        <v>111</v>
+      </c>
+      <c r="C40" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B41" t="s">
+        <v>112</v>
+      </c>
+      <c r="C41" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B42" t="s">
+        <v>4</v>
+      </c>
+      <c r="C42" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B43" t="s">
+        <v>8</v>
+      </c>
+      <c r="C43" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B44" t="s">
+        <v>9</v>
+      </c>
+      <c r="C44" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B45" t="s">
+        <v>106</v>
+      </c>
+      <c r="C45" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B46" t="s">
+        <v>107</v>
+      </c>
+      <c r="C46" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B47" t="s">
+        <v>108</v>
+      </c>
+      <c r="C47" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B48" t="s">
+        <v>109</v>
+      </c>
+      <c r="C48" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B49" t="s">
+        <v>110</v>
+      </c>
+      <c r="C49" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B50" t="s">
+        <v>111</v>
+      </c>
+      <c r="C50" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B51" t="s">
+        <v>112</v>
+      </c>
+      <c r="C51" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B52" t="s">
+        <v>4</v>
+      </c>
+      <c r="C52" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B53" t="s">
+        <v>8</v>
+      </c>
+      <c r="C53" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B54" t="s">
+        <v>9</v>
+      </c>
+      <c r="C54" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B55" t="s">
+        <v>106</v>
+      </c>
+      <c r="C55" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B56" t="s">
+        <v>107</v>
+      </c>
+      <c r="C56" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B57" t="s">
+        <v>108</v>
+      </c>
+      <c r="C57" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B58" t="s">
+        <v>109</v>
+      </c>
+      <c r="C58" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B59" t="s">
+        <v>110</v>
+      </c>
+      <c r="C59" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B60" t="s">
+        <v>111</v>
+      </c>
+      <c r="C60" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B61" t="s">
+        <v>112</v>
+      </c>
+      <c r="C61" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B62" t="s">
+        <v>4</v>
+      </c>
+      <c r="C62" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B63" t="s">
+        <v>8</v>
+      </c>
+      <c r="C63" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B64" t="s">
+        <v>9</v>
+      </c>
+      <c r="C64" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B65" t="s">
+        <v>106</v>
+      </c>
+      <c r="C65" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B66" t="s">
+        <v>107</v>
+      </c>
+      <c r="C66" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B67" t="s">
+        <v>108</v>
+      </c>
+      <c r="C67" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B68" t="s">
+        <v>109</v>
+      </c>
+      <c r="C68" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B69" t="s">
+        <v>110</v>
+      </c>
+      <c r="C69" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A70" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B70" t="s">
+        <v>111</v>
+      </c>
+      <c r="C70" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B71" t="s">
+        <v>112</v>
+      </c>
+      <c r="C71" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A72" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B72" t="s">
+        <v>4</v>
+      </c>
+      <c r="C72" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A73" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B73" t="s">
+        <v>8</v>
+      </c>
+      <c r="C73" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A74" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B74" t="s">
+        <v>9</v>
+      </c>
+      <c r="C74" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A75" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B75" t="s">
+        <v>106</v>
+      </c>
+      <c r="C75" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A76" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B76" t="s">
+        <v>107</v>
+      </c>
+      <c r="C76" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A77" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B77" t="s">
+        <v>108</v>
+      </c>
+      <c r="C77" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A78" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B78" t="s">
+        <v>109</v>
+      </c>
+      <c r="C78" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A79" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B79" t="s">
+        <v>110</v>
+      </c>
+      <c r="C79" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A80" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B80" t="s">
+        <v>111</v>
+      </c>
+      <c r="C80" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A81" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B81" t="s">
+        <v>112</v>
+      </c>
+      <c r="C81" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A82" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B82" t="s">
+        <v>4</v>
+      </c>
+      <c r="C82" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A83" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B83" t="s">
+        <v>8</v>
+      </c>
+      <c r="C83" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A84" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B84" t="s">
+        <v>9</v>
+      </c>
+      <c r="C84" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A85" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B85" t="s">
+        <v>106</v>
+      </c>
+      <c r="C85" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A86" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B86" t="s">
+        <v>107</v>
+      </c>
+      <c r="C86" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A87" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B87" t="s">
+        <v>108</v>
+      </c>
+      <c r="C87" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A88" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B88" t="s">
+        <v>109</v>
+      </c>
+      <c r="C88" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A89" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B89" t="s">
+        <v>110</v>
+      </c>
+      <c r="C89" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A90" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B90" t="s">
+        <v>111</v>
+      </c>
+      <c r="C90" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A91" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B91" t="s">
+        <v>112</v>
+      </c>
+      <c r="C91" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A92" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B92" t="s">
+        <v>4</v>
+      </c>
+      <c r="C92" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A93" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B93" t="s">
+        <v>8</v>
+      </c>
+      <c r="C93" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A94" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B94" t="s">
+        <v>9</v>
+      </c>
+      <c r="C94" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A95" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B95" t="s">
+        <v>106</v>
+      </c>
+      <c r="C95" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A96" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B96" t="s">
+        <v>107</v>
+      </c>
+      <c r="C96" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A97" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B97" t="s">
+        <v>108</v>
+      </c>
+      <c r="C97" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A98" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B98" t="s">
+        <v>109</v>
+      </c>
+      <c r="C98" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A99" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B99" t="s">
+        <v>110</v>
+      </c>
+      <c r="C99" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A100" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B100" t="s">
+        <v>111</v>
+      </c>
+      <c r="C100" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A101" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B101" t="s">
+        <v>112</v>
+      </c>
+      <c r="C101" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>